<commit_message>
Updated focus in cm_fibo.xlsx
</commit_message>
<xml_diff>
--- a/py_cost_model/cm_fibo.xlsx
+++ b/py_cost_model/cm_fibo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svgr2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sven1\svgr\workspaces\python\cs4bigdata\py_cost_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A26807-3D44-45B6-A0FA-6418B0B20E99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92F19FA-7140-457F-A2E3-34EFE1A135D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="525" windowWidth="26610" windowHeight="14505" xr2:uid="{3D05C1F5-CD59-4319-ABF3-50ACF5662A96}"/>
+    <workbookView xWindow="2190" yWindow="1095" windowWidth="26610" windowHeight="14505" xr2:uid="{3D05C1F5-CD59-4319-ABF3-50ACF5662A96}"/>
   </bookViews>
   <sheets>
     <sheet name="Fibonacci Complexity" sheetId="2" r:id="rId1"/>
@@ -1156,9 +1156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6E5E14-1DC1-4121-9765-1688384EFB5D}">
   <dimension ref="A1:N1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2162,7 +2160,7 @@
         <v>4870846.9999997942</v>
       </c>
       <c r="E36" s="10">
-        <f t="shared" ref="E36:E67" si="5">(1-D$2)^A36</f>
+        <f t="shared" ref="E36:E54" si="5">(1-D$2)^A36</f>
         <v>2.0530310231465773E-7</v>
       </c>
       <c r="F36" s="13">

</xml_diff>